<commit_message>
Updated MoM Meet Report and StatusTracker3.xlsx for week(11feb-18feb)
</commit_message>
<xml_diff>
--- a/docs/StatusTracker3.xlsx
+++ b/docs/StatusTracker3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SG2PEPF00038017\EXCELCNV\842fdef7-d1bf-4243-a8a9-d23c8929deb8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B87A2EF-14DA-43FC-B75F-765971C4F7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{457933F5-2532-4E3D-872F-1A08A2F39857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -376,6 +376,9 @@
     <t>3 to 5</t>
   </si>
   <si>
+    <t>Delayed a bit but willl try to cover before R1</t>
+  </si>
+  <si>
     <t>Webscrapping data from client's website</t>
   </si>
   <si>
@@ -385,7 +388,7 @@
     <t>1 to 2</t>
   </si>
   <si>
-    <t>Week 4 (January 29 - February 4)</t>
+    <t>Week 4 (February 4-February 11)</t>
   </si>
   <si>
     <t>clarrifications on scope and requirements</t>
@@ -397,7 +400,7 @@
     <t>Samarth,Kuvam</t>
   </si>
   <si>
-    <t>Did post autmation but yet to fix the image resolution issue</t>
+    <t>Did post autmation but yet to fix the image resolution issue(Done)</t>
   </si>
   <si>
     <t>Delayed</t>
@@ -406,7 +409,7 @@
     <t>Stuck on how to get acess token(we dont have any buisness account to get one). Need to disccuss</t>
   </si>
   <si>
-    <t>Week 5</t>
+    <t>Week 5 (February 11-February 18)</t>
   </si>
   <si>
     <t xml:space="preserve">Designing of Database </t>
@@ -434,6 +437,24 @@
   </si>
   <si>
     <t>Story Automation on Instagram using Node js</t>
+  </si>
+  <si>
+    <t>Post Automation on Instagram using Node js</t>
+  </si>
+  <si>
+    <t>Done with  post automation on Instagram(FB left)</t>
+  </si>
+  <si>
+    <t>Database creation and population</t>
+  </si>
+  <si>
+    <t>Website design and developement for client approval</t>
+  </si>
+  <si>
+    <t>Done with design will start to code it up</t>
+  </si>
+  <si>
+    <t>documentation and notion page updation</t>
   </si>
   <si>
     <t>Week 6</t>
@@ -1322,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I239"/>
+  <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -1418,11 +1439,11 @@
       <c r="F7" s="15"/>
       <c r="G7" s="2"/>
       <c r="H7" s="12" t="str">
-        <f t="shared" ref="H7:H76" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
+        <f t="shared" ref="H7:H80" si="0">IF(OR(D7="", E7=""), "", D7-E7)</f>
         <v/>
       </c>
       <c r="I7" s="12" t="str">
-        <f t="shared" ref="I7:I76" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
+        <f t="shared" ref="I7:I80" si="1">IF(OR(H7="",E7=0),"",ABS(H7)/E7*100)</f>
         <v/>
       </c>
     </row>
@@ -1611,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
         <v>58</v>
@@ -2012,7 +2033,7 @@
         <v>80</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="H31" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2039,6 +2060,9 @@
       <c r="F32" s="16" t="s">
         <v>53</v>
       </c>
+      <c r="G32" t="s">
+        <v>83</v>
+      </c>
       <c r="H32" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2050,16 +2074,16 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
         <v>79</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E33" s="5">
         <v>1.5</v>
@@ -2094,7 +2118,7 @@
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="4"/>
@@ -2131,7 +2155,7 @@
         <v>40</v>
       </c>
       <c r="G36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H36" s="12">
         <f t="shared" si="0"/>
@@ -2166,22 +2190,22 @@
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="27" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B38" t="s">
         <v>79</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>67</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="G38" s="27" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H38" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2200,20 +2224,20 @@
         <v>79</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G39" s="27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H39" s="12"/>
       <c r="I39" s="12"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="10"/>
@@ -2232,22 +2256,22 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="27" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B41" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="F41" s="16" t="s">
         <v>53</v>
       </c>
       <c r="G41" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H41" s="12" t="str">
         <f t="shared" si="0"/>
@@ -2260,7 +2284,7 @@
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="27" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
         <v>38</v>
@@ -2278,7 +2302,7 @@
         <v>40</v>
       </c>
       <c r="G42" s="27" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H42" s="12">
         <f t="shared" si="0"/>
@@ -2291,7 +2315,7 @@
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="27" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B43" t="s">
         <v>79</v>
@@ -2309,7 +2333,7 @@
         <v>40</v>
       </c>
       <c r="G43" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H43" s="12">
         <f t="shared" si="0"/>
@@ -2322,13 +2346,13 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="27" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B44" t="s">
         <v>79</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D44" s="5">
         <v>1.5</v>
@@ -2343,55 +2367,108 @@
       <c r="I44" s="12"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="B45" s="2"/>
-      <c r="C45" s="10"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="2"/>
-      <c r="H45" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I45" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A45" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" s="5">
+        <v>1</v>
+      </c>
+      <c r="E45" s="5">
+        <v>1</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="H46" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I46" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A46" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F46" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G46" s="27"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="H47" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I47" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
+      <c r="A47" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" s="5">
+        <v>1</v>
+      </c>
+      <c r="E47" s="5">
+        <v>1</v>
+      </c>
+      <c r="F47" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="H47" s="12"/>
+      <c r="I47" s="12"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="H48" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I48" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="8:9">
+      <c r="A48" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48" s="5">
+        <v>1</v>
+      </c>
+      <c r="E48" s="5">
+        <v>1</v>
+      </c>
+      <c r="F48" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G48" s="27"/>
+      <c r="H48" s="12"/>
+      <c r="I48" s="12"/>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="2"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="2"/>
       <c r="H49" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2401,7 +2478,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="8:9">
+    <row r="50" spans="1:9">
       <c r="H50" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2411,7 +2488,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="8:9">
+    <row r="51" spans="1:9">
       <c r="H51" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2421,7 +2498,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="8:9">
+    <row r="52" spans="1:9">
       <c r="H52" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2431,7 +2508,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="8:9">
+    <row r="53" spans="1:9">
       <c r="H53" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2441,7 +2518,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="8:9">
+    <row r="54" spans="1:9">
       <c r="H54" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2451,7 +2528,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="8:9">
+    <row r="55" spans="1:9">
       <c r="H55" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2461,7 +2538,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="8:9">
+    <row r="56" spans="1:9">
       <c r="H56" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2471,7 +2548,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="8:9">
+    <row r="57" spans="1:9">
       <c r="H57" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2481,7 +2558,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="8:9">
+    <row r="58" spans="1:9">
       <c r="H58" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2491,7 +2568,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="8:9">
+    <row r="59" spans="1:9">
       <c r="H59" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2501,7 +2578,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="8:9">
+    <row r="60" spans="1:9">
       <c r="H60" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2511,7 +2588,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="8:9">
+    <row r="61" spans="1:9">
       <c r="H61" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2521,7 +2598,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="8:9">
+    <row r="62" spans="1:9">
       <c r="H62" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2531,7 +2608,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="8:9">
+    <row r="63" spans="1:9">
       <c r="H63" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2541,7 +2618,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="8:9">
+    <row r="64" spans="1:9">
       <c r="H64" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2673,51 +2750,51 @@
     </row>
     <row r="77" spans="8:9">
       <c r="H77" s="12" t="str">
-        <f t="shared" ref="H77:H140" si="2">IF(OR(D77="", E77=""), "", D77-E77)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I77" s="12" t="str">
-        <f t="shared" ref="I77:I140" si="3">IF(OR(H77="",E77=0),"",ABS(H77)/E77*100)</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="8:9">
       <c r="H78" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I78" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="8:9">
       <c r="H79" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I79" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="8:9">
       <c r="H80" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="I80" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="8:9">
       <c r="H81" s="12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H81:H144" si="2">IF(OR(D81="", E81=""), "", D81-E81)</f>
         <v/>
       </c>
       <c r="I81" s="12" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I81:I144" si="3">IF(OR(H81="",E81=0),"",ABS(H81)/E81*100)</f>
         <v/>
       </c>
     </row>
@@ -3313,51 +3390,51 @@
     </row>
     <row r="141" spans="8:9">
       <c r="H141" s="12" t="str">
-        <f t="shared" ref="H141:H204" si="4">IF(OR(D141="", E141=""), "", D141-E141)</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I141" s="12" t="str">
-        <f t="shared" ref="I141:I204" si="5">IF(OR(H141="",E141=0),"",ABS(H141)/E141*100)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="142" spans="8:9">
       <c r="H142" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I142" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="143" spans="8:9">
       <c r="H143" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I143" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="144" spans="8:9">
       <c r="H144" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I144" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
     </row>
     <row r="145" spans="8:9">
       <c r="H145" s="12" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H145:H208" si="4">IF(OR(D145="", E145=""), "", D145-E145)</f>
         <v/>
       </c>
       <c r="I145" s="12" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I145:I208" si="5">IF(OR(H145="",E145=0),"",ABS(H145)/E145*100)</f>
         <v/>
       </c>
     </row>
@@ -3953,51 +4030,51 @@
     </row>
     <row r="205" spans="8:9">
       <c r="H205" s="12" t="str">
-        <f t="shared" ref="H205:H232" si="6">IF(OR(D205="", E205=""), "", D205-E205)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I205" s="12" t="str">
-        <f t="shared" ref="I205:I239" si="7">IF(OR(H205="",E205=0),"",ABS(H205)/E205*100)</f>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="206" spans="8:9">
       <c r="H206" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I206" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="207" spans="8:9">
       <c r="H207" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I207" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="208" spans="8:9">
       <c r="H208" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I208" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
     <row r="209" spans="8:9">
       <c r="H209" s="12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H209:H236" si="6">IF(OR(D209="", E209=""), "", D209-E209)</f>
         <v/>
       </c>
       <c r="I209" s="12" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="I209:I243" si="7">IF(OR(H209="",E209=0),"",ABS(H209)/E209*100)</f>
         <v/>
       </c>
     </row>
@@ -4232,24 +4309,40 @@
       </c>
     </row>
     <row r="233" spans="8:9">
+      <c r="H233" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I233" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="234" spans="8:9">
+      <c r="H234" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I234" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="235" spans="8:9">
+      <c r="H235" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I235" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="236" spans="8:9">
+      <c r="H236" s="12" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I236" s="12" t="str">
         <f t="shared" si="7"/>
         <v/>
@@ -4273,9 +4366,33 @@
         <v/>
       </c>
     </row>
+    <row r="240" spans="8:9">
+      <c r="I240" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="241" spans="9:9">
+      <c r="I241" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="242" spans="9:9">
+      <c r="I242" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="243" spans="9:9">
+      <c r="I243" s="12" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
-  <conditionalFormatting sqref="F29:F39 F41:F44 F46:F65519 F5:F27">
+  <conditionalFormatting sqref="F29:F39 F41:F48 F50:F65523 F5:F27">
     <cfRule type="cellIs" dxfId="11" priority="31" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>
@@ -4308,7 +4425,7 @@
       <formula>"Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F45">
+  <conditionalFormatting sqref="F49">
     <cfRule type="cellIs" dxfId="2" priority="22" stopIfTrue="1" operator="equal">
       <formula>"Delayed"</formula>
     </cfRule>
@@ -4320,10 +4437,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F65519" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F65523" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Planned, Ongoing, Delayed, Done"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B65519" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B65523" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Requirements, Design, Development, Testing, Preparation, Coordination, Documentation, Interfaces, Delivery"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated mom and status-tracker
</commit_message>
<xml_diff>
--- a/docs/StatusTracker3.xlsx
+++ b/docs/StatusTracker3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\SG2PEPF00038017\EXCELCNV\842fdef7-d1bf-4243-a8a9-d23c8929deb8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{457933F5-2532-4E3D-872F-1A08A2F39857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{51C1F5ED-F9CA-476F-9A58-8A6786DDFB16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="125">
   <si>
     <t>Using the Status tracker</t>
   </si>
@@ -457,7 +457,49 @@
     <t>documentation and notion page updation</t>
   </si>
   <si>
-    <t>Week 6</t>
+    <t>Week 6(February 18-February 25)</t>
+  </si>
+  <si>
+    <t>SRS documentation</t>
+  </si>
+  <si>
+    <t>Server developement</t>
+  </si>
+  <si>
+    <t>Anna,Tanay,Samarth</t>
+  </si>
+  <si>
+    <t>3 to 6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Building a server to make allow client-server-db interaction </t>
+  </si>
+  <si>
+    <t>Edit Functionality on Website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allows client to edit the caption </t>
+  </si>
+  <si>
+    <t>Approve functionality on Website</t>
+  </si>
+  <si>
+    <t>Allows client to approve a template to  be posted</t>
+  </si>
+  <si>
+    <t>Caption production using Chat-gpt-Api</t>
+  </si>
+  <si>
+    <t>Client approval left</t>
+  </si>
+  <si>
+    <t>Test-plan-tracker</t>
+  </si>
+  <si>
+    <t>static webpage developement</t>
+  </si>
+  <si>
+    <t>Reject Functionality on Website</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" outlineLevelRow="2"/>
@@ -2479,26 +2521,80 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="H50" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I50" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A50" t="s">
+        <v>111</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E50" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F50" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I50" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="H51" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I51" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A51" t="s">
+        <v>73</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5">
+        <v>1</v>
+      </c>
+      <c r="F51" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H51" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:9">
+      <c r="A52" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="F52" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G52" t="s">
+        <v>115</v>
+      </c>
       <c r="H52" s="12" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2509,63 +2605,180 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="H53" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I53" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A53" t="s">
+        <v>116</v>
+      </c>
+      <c r="B53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D53" s="5">
+        <v>1</v>
+      </c>
+      <c r="E53" s="5">
+        <v>1</v>
+      </c>
+      <c r="F53" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G53" t="s">
+        <v>117</v>
+      </c>
+      <c r="H53" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I53" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="H54" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I54" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A54" t="s">
+        <v>118</v>
+      </c>
+      <c r="B54" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D54" s="5">
+        <v>1</v>
+      </c>
+      <c r="E54" s="5">
+        <v>1</v>
+      </c>
+      <c r="F54" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" t="s">
+        <v>119</v>
+      </c>
+      <c r="H54" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="H55" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I55" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A55" t="s">
+        <v>120</v>
+      </c>
+      <c r="B55" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="5">
+        <v>1</v>
+      </c>
+      <c r="E55" s="5">
+        <v>1</v>
+      </c>
+      <c r="F55" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="G55" t="s">
+        <v>121</v>
+      </c>
+      <c r="H55" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I55" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="H56" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I56" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A56" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" s="5">
+        <v>2</v>
+      </c>
+      <c r="E56" s="5">
+        <v>2</v>
+      </c>
+      <c r="F56" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H56" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I56" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="H57" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I57" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A57" t="s">
+        <v>123</v>
+      </c>
+      <c r="B57" t="s">
+        <v>79</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="E57" s="5">
+        <v>2</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H57" s="12">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
+      <c r="I57" s="12">
+        <f t="shared" si="1"/>
+        <v>25</v>
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="H58" s="12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I58" s="12" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="A58" t="s">
+        <v>124</v>
+      </c>
+      <c r="B58" t="s">
+        <v>79</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D58" s="5">
+        <v>1</v>
+      </c>
+      <c r="E58" s="5">
+        <v>1</v>
+      </c>
+      <c r="F58" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I58" s="12">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:9">

</xml_diff>

<commit_message>
Updated all docs for R1
</commit_message>
<xml_diff>
--- a/docs/StatusTracker3.xlsx
+++ b/docs/StatusTracker3.xlsx
@@ -317,7 +317,7 @@
       <style:text-properties fo:color="#000000" loext:opacity="100%" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:text-position="0% 100%" fo:font-family="Tahoma" style:font-family-generic="swiss" fo:font-size="8pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="8pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-family-complex="Tahoma" style:font-family-generic-complex="swiss" style:font-size-complex="8pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="bold" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color" fo:hyphenate="false"/>
     </style:style>
     <style:style style:name="T1" style:family="text">
-      <style:text-properties style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+      <style:text-properties fo:color="#000000" loext:opacity="100%" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:text-position="0% 100%" style:font-name="Arial" fo:font-size="10pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
     <style:style style:name="T2" style:family="text">
       <style:text-properties fo:color="#000000" loext:opacity="100%" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:text-position="0% 100%" fo:font-family="Tahoma" style:font-family-generic="swiss" fo:font-size="8pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="8pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-family-complex="Tahoma" style:font-family-generic-complex="swiss" style:font-size-complex="8pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
@@ -2091,7 +2091,7 @@
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
-            <text:p>Ongoing</text:p>
+            <text:p>Done</text:p>
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D66]=&quot;&quot;; [.E66]=&quot;&quot;); &quot;&quot;; [.D66]-[.E66])">
@@ -2238,11 +2238,13 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
+          <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
+            <text:p>Week 8(March 10-March 16)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce48" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
+          <table:table-cell table:style-name="ce48"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D72]=&quot;&quot;; [.E72]=&quot;&quot;); &quot;&quot;; [.D72]-[.E72])">
             <text:p/>
           </table:table-cell>
@@ -2252,24 +2254,50 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D73]=&quot;&quot;; [.E73]=&quot;&quot;); &quot;&quot;; [.D73]-[.E73])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H73]=&quot;&quot;;[.E73]=0);&quot;&quot;;ABS([.H73])/[.E73]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Sever Deployemnt</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce61" office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D73]=&quot;&quot;; [.E73]=&quot;&quot;); &quot;&quot;; [.D73]-[.E73])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H73]=&quot;&quot;;[.E73]=0);&quot;&quot;;ABS([.H73])/[.E73]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Research on WebCrawling </text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Kuvam,Anna</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce25" office:value-type="date" office:date-value="2024-04-03" calcext:value-type="date">
+            <text:p>03/04/24</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D74]=&quot;&quot;; [.E74]=&quot;&quot;); &quot;&quot;; [.D74]-[.E74])">
             <text:p/>
@@ -2280,51 +2308,94 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D75]=&quot;&quot;; [.E75]=&quot;&quot;); &quot;&quot;; [.D75]-[.E75])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H75]=&quot;&quot;;[.E75]=0);&quot;&quot;;ABS([.H75])/[.E75]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D76]=&quot;&quot;; [.E76]=&quot;&quot;); &quot;&quot;; [.D76]-[.E76])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H76]=&quot;&quot;;[.E76]=0);&quot;&quot;;ABS([.H76])/[.E76]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D77]=&quot;&quot;; [.E77]=&quot;&quot;); &quot;&quot;; [.D77]-[.E77])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H77]=&quot;&quot;;[.E77]=0);&quot;&quot;;ABS([.H77])/[.E77]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Client meeting</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Coordination</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce61" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D75]=&quot;&quot;; [.E75]=&quot;&quot;); &quot;&quot;; [.D75]-[.E75])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H75]=&quot;&quot;;[.E75]=0);&quot;&quot;;ABS([.H75])/[.E75]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>R1 PPT </text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Documentation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Vidhi</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>1 to 2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2.5" calcext:value-type="float">
+            <text:p>2.5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D76]=&quot;&quot;; [.E76]=&quot;&quot;); &quot;&quot;; [.D76]-[.E76])" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H76]=&quot;&quot;;[.E76]=0);&quot;&quot;;ABS([.H76])/[.E76]*100)" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Github Workflow Implimentation</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D77]=&quot;&quot;; [.E77]=&quot;&quot;); &quot;&quot;; [.D77]-[.E77])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H77]=&quot;&quot;;[.E77]=0);&quot;&quot;;ABS([.H77])/[.E77]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Design</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce25"/>
+          <table:table-cell/>
           <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D78]=&quot;&quot;; [.E78]=&quot;&quot;); &quot;&quot;; [.D78]-[.E78])">
@@ -4671,11 +4742,11 @@
   <office:meta>
     <meta:initial-creator>swami</meta:initial-creator>
     <meta:creation-date>2003-08-12T18:15:36</meta:creation-date>
-    <dc:date>2024-03-15T00:11:33.649955041</dc:date>
+    <dc:date>2024-03-19T23:35:51.506009158</dc:date>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
-    <meta:editing-duration>PT16M29S</meta:editing-duration>
-    <meta:editing-cycles>2</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="835" meta:object-count="0"/>
+    <meta:editing-duration>PT18M8S</meta:editing-duration>
+    <meta:editing-cycles>3</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="866" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">16.0300</meta:user-defined>
     <meta:user-defined meta:name="Company">RIT</meta:user-defined>
   </office:meta>
@@ -4710,12 +4781,12 @@
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Status">
               <config:config-item config:name="CursorPositionX" config:type="int">6</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">70</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">77</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">24</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">37</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">14</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -4780,7 +4851,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">lAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAtQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">oAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -4825,111 +4896,111 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
+    <number:number-style style:name="N126">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
+    <number:number-style style:name="N125P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+    </number:number-style>
+    <number:number-style style:name="N125">
+      <number:text>-</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N125P0"/>
+    </number:number-style>
     <number:number-style style:name="N123P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
     <number:number-style style:name="N123">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N123P0"/>
     </number:number-style>
-    <number:number-style style:name="N122P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
+    <number:time-style style:name="N122" number:truncate-on-overflow="false">
+      <number:hours/>
+      <number:text>:</number:text>
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N121P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N122P1" style:volatile="true">
+    <number:number-style style:name="N121">
       <number:text>-</number:text>
-      <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
     </number:number-style>
-    <number:number-style style:name="N122P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N122">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N122P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N122P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N122P2"/>
-    </number:text-style>
-    <number:number-style style:name="N118P0" style:volatile="true">
+    <number:time-style style:name="N120">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
+    <number:number-style style:name="N119P0" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N118P1" style:volatile="true">
+    <number:number-style style:name="N119P1" style:volatile="true">
       <number:text>-</number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N118P2" style:volatile="true">
+    <number:number-style style:name="N119P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N118">
+    <number:text-style style:name="N119">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N118P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N118P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N118P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N119P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N119P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N119P2"/>
     </number:text-style>
-    <number:time-style style:name="N114">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N126P0" style:volatile="true">
+    <number:number-style style:name="N115P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N126">
+    <number:number-style style:name="N115P1" style:volatile="true">
       <number:text>-</number:text>
+      <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N126P0"/>
+      <number:text> </number:text>
     </number:number-style>
-    <number:time-style style:name="N113" number:truncate-on-overflow="false">
-      <number:hours/>
-      <number:text>:</number:text>
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N125P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+    <number:number-style style:name="N115P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
     </number:number-style>
-    <number:number-style style:name="N125">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N125P0"/>
-    </number:number-style>
-    <number:time-style style:name="N112">
+    <number:text-style style:name="N115">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N115P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N115P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N115P2"/>
+    </number:text-style>
+    <number:time-style style:name="N124">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long" number:decimal-places="1"/>
     </number:time-style>
-    <number:number-style style:name="N124P0" style:volatile="true">
+    <number:number-style style:name="N111P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N124">
+    <number:number-style style:name="N111">
+      <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N124P0"/>
-    </number:number-style>
-    <number:number-style style:name="N111">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N111P0"/>
     </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
       <style:table-cell-properties style:rotation-align="none" style:vertical-align="bottom"/>
@@ -5089,7 +5160,7 @@
         <style:region-right>
           <text:p>
             <text:span text:style-name="MT1">
-              <text:date style:data-style-name="N2" text:date-value="2024-03-15">00/00/0000</text:date>
+              <text:date style:data-style-name="N2" text:date-value="2024-03-19">00/00/0000</text:date>
             </text:span>
           </text:p>
         </style:region-right>

</xml_diff>

<commit_message>
updated MOM and status_tracker
</commit_message>
<xml_diff>
--- a/docs/StatusTracker3.xlsx
+++ b/docs/StatusTracker3.xlsx
@@ -112,6 +112,18 @@
       <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
     <style:style style:name="ce13" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
+      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
+    </style:style>
+    <style:style style:name="ce40" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:rotation-align="none"/>
+      <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
+    </style:style>
+    <style:style style:name="ce41" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties style:rotation-align="none"/>
+      <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
+    </style:style>
+    <style:style style:name="ce42" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#969696" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
@@ -129,7 +141,7 @@
       <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce43" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce47" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#969696" style:rotation-align="none"/>
     </style:style>
     <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default">
@@ -140,17 +152,24 @@
       <style:table-cell-properties fo:background-color="#999999"/>
       <style:text-properties style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="10pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="bold" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
     </style:style>
+    <style:style style:name="ce46" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#808080"/>
+      <style:text-properties style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial" fo:font-size="10pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="10pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial" style:font-size-complex="10pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="bold" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
     <style:style style:name="ce11" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:rotation-align="none"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce47" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce52" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fcf305" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="12pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="12pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="12pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce48" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce53" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#999999"/>
+    </style:style>
+    <style:style style:name="ce54" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#808080"/>
     </style:style>
     <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#969696" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
@@ -183,6 +202,10 @@
     </style:style>
     <style:style style:name="ce20" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#999999" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
+      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
+    </style:style>
+    <style:style style:name="ce58" style:family="table-cell" style:parent-style-name="Default">
+      <style:table-cell-properties fo:background-color="#808080" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
     </style:style>
     <style:style style:name="ce21" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
@@ -269,6 +292,13 @@
     </style:style>
     <style:style style:name="ce34" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
       <style:table-cell-properties fo:background-color="#999999" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
+      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
+      <style:map style:condition="cell-content()=&quot;Delayed&quot;" style:apply-style-name="ConditionalStyle_5f_12" style:base-cell-address="Status.F5"/>
+      <style:map style:condition="cell-content()=&quot;Done&quot;" style:apply-style-name="ConditionalStyle_5f_11" style:base-cell-address="Status.F5"/>
+      <style:map style:condition="cell-content()=&quot;Ongoing&quot;" style:apply-style-name="ConditionalStyle_5f_10" style:base-cell-address="Status.F5"/>
+    </style:style>
+    <style:style style:name="ce75" style:family="table-cell" style:parent-style-name="Default" style:data-style-name="N100">
+      <style:table-cell-properties fo:background-color="#808080" style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
       <style:map style:condition="cell-content()=&quot;Delayed&quot;" style:apply-style-name="ConditionalStyle_5f_12" style:base-cell-address="Status.F5"/>
       <style:map style:condition="cell-content()=&quot;Done&quot;" style:apply-style-name="ConditionalStyle_5f_11" style:base-cell-address="Status.F5"/>
@@ -344,17 +374,17 @@
         <table:table-column table:style-name="co2" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co3" table:number-columns-repeated="1022" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce1"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce13"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce40" office:value-type="string" calcext:value-type="string">
             <text:p>Using the Status tracker</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1021"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
-          <table:table-cell table:style-name="ce1"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce2"/>
+          <table:table-cell table:style-name="ce13"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce40"/>
           <table:table-cell table:number-columns-repeated="1021"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
@@ -437,72 +467,72 @@
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" office:value-type="string" calcext:value-type="string">
             <text:p>PROJECT NUMBER</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>(Fill your Project Number here)</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" office:value-type="string" calcext:value-type="string">
             <text:p>PROJECT NAME</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>(Fill your project name here)</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" office:value-type="string" calcext:value-type="string">
             <text:p>PROJECT MENTOR (sponsor)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>(Put your Project Mentor (sponsor) name here)</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro5">
-          <table:table-cell table:style-name="ce2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" office:value-type="string" calcext:value-type="string">
             <text:p>TEAM MEMBERS</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>Team Mamber Name 1</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>Team Member Name 2</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>Team Member Name 3</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>Team Member Name 4</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce41" office:value-type="string" calcext:value-type="string">
             <text:p>Team Member Name 5</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell/>
-          <table:table-cell table:style-name="ce3"/>
+          <table:table-cell table:style-name="ce41"/>
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro2" table:number-rows-repeated="1048548">
@@ -516,15 +546,15 @@
         <office:forms form:automatic-focus="false" form:apply-design-mode="false"/>
         <table:table-column table:style-name="co4" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co5" table:default-cell-style-name="Default"/>
-        <table:table-column table:style-name="co6" table:default-cell-style-name="ce1"/>
-        <table:table-column table:style-name="co7" table:default-cell-style-name="ce1"/>
-        <table:table-column table:style-name="co8" table:default-cell-style-name="ce1"/>
+        <table:table-column table:style-name="co6" table:default-cell-style-name="ce13"/>
+        <table:table-column table:style-name="co7" table:default-cell-style-name="ce13"/>
+        <table:table-column table:style-name="co8" table:default-cell-style-name="ce13"/>
         <table:table-column table:style-name="co9" table:default-cell-style-name="ce26"/>
         <table:table-column table:style-name="co10" table:default-cell-style-name="Default"/>
         <table:table-column table:style-name="co8" table:number-columns-repeated="2" table:default-cell-style-name="ce35"/>
         <table:table-column table:style-name="co3" table:number-columns-repeated="1015" table:default-cell-style-name="Default"/>
         <table:table-row table:style-name="ro6">
-          <table:table-cell table:style-name="ce2" table:formula="of:=([$Instructions.A19])" office:value-type="string" office:string-value="PROJECT NUMBER" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" table:formula="of:=([$Instructions.A19])" office:value-type="string" office:string-value="PROJECT NUMBER" calcext:value-type="string">
             <text:p>PROJECT NUMBER</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce11" office:value-type="float" office:value="2" calcext:value-type="float">
@@ -533,7 +563,7 @@
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro4">
-          <table:table-cell table:style-name="ce2" table:formula="of:=([$Instructions.A20])" office:value-type="string" office:string-value="PROJECT NAME" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" table:formula="of:=([$Instructions.A20])" office:value-type="string" office:string-value="PROJECT NAME" calcext:value-type="string">
             <text:p>PROJECT NAME</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce11" office:value-type="string" calcext:value-type="string">
@@ -542,7 +572,7 @@
           <table:table-cell table:number-columns-repeated="1022"/>
         </table:table-row>
         <table:table-row table:style-name="ro3">
-          <table:table-cell table:style-name="ce2" table:formula="of:=([$Instructions.A21])" office:value-type="string" office:string-value="PROJECT MENTOR (sponsor)" calcext:value-type="string">
+          <table:table-cell table:style-name="ce40" table:formula="of:=([$Instructions.A21])" office:value-type="string" office:string-value="PROJECT MENTOR (sponsor)" calcext:value-type="string">
             <text:p>PROJECT MENTOR (sponsor)</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce11" office:value-type="string" calcext:value-type="string">
@@ -554,10 +584,10 @@
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro7">
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce42" office:value-type="string" calcext:value-type="string">
             <text:p>Activity Name</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce13" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce42" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
             <text:p>Type</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
@@ -581,7 +611,7 @@
           <table:table-cell table:style-name="ce27" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
             <text:p>Status</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce13" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce42" office:value-type="string" calcext:value-type="string">
             <office:annotation draw:style-name="gr2" draw:text-style-name="P2" svg:width="2.857cm" svg:height="1.252cm" svg:x="28.489cm" svg:y="3.73cm" draw:caption-point-x="4.957cm" draw:caption-point-y="-0.413cm">
               <dc:date>2024-03-01T00:00:00</dc:date>
               <text:p text:style-name="P1">
@@ -618,12 +648,12 @@
                   <text:a xlink:href="#Instructions.A1" xlink:type="simple">    See Instructions sheet for usage</text:a>
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce52" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce15" table:number-columns-repeated="3"/>
               <table:table-cell table:style-name="ce28" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce47"/>
+              <table:table-cell table:style-name="ce52"/>
               <table:table-cell table:style-name="ce15" table:number-columns-repeated="2"/>
-              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce52" table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
               <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
@@ -633,11 +663,11 @@
                   January 21)
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce22" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce43"/>
+              <table:table-cell table:style-name="ce47"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D7]=&quot;&quot;; [.E7]=&quot;&quot;); &quot;&quot;; [.D7]-[.E7])">
                 <text:p/>
               </table:table-cell>
@@ -891,18 +921,18 @@
                   28)
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce43"/>
+              <table:table-cell table:style-name="ce47"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D17]=&quot;&quot;; [.E17]=&quot;&quot;); &quot;&quot;; [.D17]-[.E17])">
                 <text:p/>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H17]=&quot;&quot;;[.E17]=0);&quot;&quot;;ABS([.H17])/[.E17]*100)">
                 <text:p/>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
               <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1061,10 +1091,10 @@
               <table:table-cell table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
-              <table:table-cell table:style-name="ce43" office:value-type="string" calcext:value-type="string">
+              <table:table-cell table:style-name="ce47" office:value-type="string" calcext:value-type="string">
                 <text:p>Status tracker</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+              <table:table-cell table:style-name="ce47" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
                 <text:p>Documentation</text:p>
               </table:table-cell>
               <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1076,14 +1106,14 @@
               <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
                 <text:p>Done</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43"/>
+              <table:table-cell table:style-name="ce47"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D24]=&quot;&quot;; [.E24]=&quot;&quot;); &quot;&quot;; [.D24]-[.E24])" office:value-type="float" office:value="0" calcext:value-type="float">
                 <text:p>0</text:p>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H24]=&quot;&quot;;[.E24]=0);&quot;&quot;;ABS([.H24])/[.E24]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
                 <text:p>0</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
             </table:table-row>
           </table:table-row-group>
         </table:table-row-group>
@@ -1146,18 +1176,18 @@
               <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
                 <text:p>Week 3 (January 29 - February 4)</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce31" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce43"/>
+              <table:table-cell table:style-name="ce47"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D28]=&quot;&quot;; [.E28]=&quot;&quot;); &quot;&quot;; [.D28]-[.E28])">
                 <text:p/>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H28]=&quot;&quot;;[.E28]=0);&quot;&quot;;ABS([.H28])/[.E28]*100)">
                 <text:p/>
               </table:table-cell>
-              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
             </table:table-row>
           </table:table-row-group>
         </table:table-row-group>
@@ -1312,12 +1342,12 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 4 (February 4-February 11)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce18"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce43"/>
+          <table:table-cell table:style-name="ce47"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D35]=&quot;&quot;; [.E35]=&quot;&quot;); &quot;&quot;; [.D35]-[.E35])">
             <text:p/>
           </table:table-cell>
@@ -1436,11 +1466,11 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 5 (February 11-February 18)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce32" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce43"/>
+          <table:table-cell table:style-name="ce47"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D40]=&quot;&quot;; [.E40]=&quot;&quot;); &quot;&quot;; [.D40]-[.E40])">
             <text:p/>
           </table:table-cell>
@@ -1648,11 +1678,11 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 6(February 18-February 25)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce33" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce43"/>
+          <table:table-cell table:style-name="ce47"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D49]=&quot;&quot;; [.E49]=&quot;&quot;); &quot;&quot;; [.D49]-[.E49])">
             <text:p/>
           </table:table-cell>
@@ -1908,10 +1938,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 7(February 25-March 2)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce48" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce48"/>
+          <table:table-cell table:style-name="ce53"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D59]=&quot;&quot;; [.E59]=&quot;&quot;); &quot;&quot;; [.D59]-[.E59])">
             <text:p/>
           </table:table-cell>
@@ -2064,10 +2094,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 8(March 2-March 9)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce48" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce48"/>
+          <table:table-cell table:style-name="ce53"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D65]=&quot;&quot;; [.E65]=&quot;&quot;); &quot;&quot;; [.D65]-[.E65])">
             <text:p/>
           </table:table-cell>
@@ -2241,10 +2271,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 8(March 10-March 16)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce48" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce48"/>
+          <table:table-cell table:style-name="ce53"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D72]=&quot;&quot;; [.E72]=&quot;&quot;); &quot;&quot;; [.D72]-[.E72])">
             <text:p/>
           </table:table-cell>
@@ -2389,90 +2419,143 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
+          <table:table-cell table:style-name="ce46" office:value-type="string" calcext:value-type="string">
+            <text:p>Week 9(March 23-March 31)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce54" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce58" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce75" table:content-validation-name="val2"/>
+          <table:table-cell table:style-name="ce54"/>
+          <table:table-cell table:style-name="ce37" table:number-columns-repeated="2"/>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Research on popular suggestive models</text:p>
+          </table:table-cell>
           <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
-            <text:p>Design</text:p>
-          </table:table-cell>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce25"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D78]=&quot;&quot;; [.E78]=&quot;&quot;); &quot;&quot;; [.D78]-[.E78])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H78]=&quot;&quot;;[.E78]=0);&quot;&quot;;ABS([.H78])/[.E78]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D79]=&quot;&quot;; [.E79]=&quot;&quot;); &quot;&quot;; [.D79]-[.E79])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H79]=&quot;&quot;;[.E79]=0);&quot;&quot;;ABS([.H79])/[.E79]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D80]=&quot;&quot;; [.E80]=&quot;&quot;); &quot;&quot;; [.D80]-[.E80])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H80]=&quot;&quot;;[.E80]=0);&quot;&quot;;ABS([.H80])/[.E80]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D81]=&quot;&quot;; [.E81]=&quot;&quot;); &quot;&quot;; [.D81]-[.E81])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H81]=&quot;&quot;;[.E81]=0);&quot;&quot;;ABS([.H81])/[.E81]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D82]=&quot;&quot;; [.E82]=&quot;&quot;); &quot;&quot;; [.D82]-[.E82])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H82]=&quot;&quot;;[.E82]=0);&quot;&quot;;ABS([.H82])/[.E82]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D83]=&quot;&quot;; [.E83]=&quot;&quot;); &quot;&quot;; [.D83]-[.E83])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H83]=&quot;&quot;;[.E83]=0);&quot;&quot;;ABS([.H83])/[.E83]*100)">
-            <text:p/>
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
+            <text:p>4</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="5" calcext:value-type="float">
+            <text:p>5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D79]=&quot;&quot;; [.E79]=&quot;&quot;); &quot;&quot;; [.D79]-[.E79])" office:value-type="float" office:value="-1" calcext:value-type="float">
+            <text:p>-1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H79]=&quot;&quot;;[.E79]=0);&quot;&quot;;ABS([.H79])/[.E79]*100)" office:value-type="float" office:value="20" calcext:value-type="float">
+            <text:p>20</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>WebCrawling for other items</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Anna,Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D80]=&quot;&quot;; [.E80]=&quot;&quot;); &quot;&quot;; [.D80]-[.E80])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H80]=&quot;&quot;;[.E80]=0);&quot;&quot;;ABS([.H80])/[.E80]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Captions Updation</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Kuvam,Tanay</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2 to 3</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Meet with Client</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Further extra features discussion</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D82]=&quot;&quot;; [.E82]=&quot;&quot;); &quot;&quot;; [.D82]-[.E82])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H82]=&quot;&quot;;[.E82]=0);&quot;&quot;;ABS([.H82])/[.E82]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Website Refinement</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Vidhi</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H83]=&quot;&quot;;[.E83]=0);&quot;&quot;;ABS([.H83])/[.E83]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
@@ -4742,11 +4825,11 @@
   <office:meta>
     <meta:initial-creator>swami</meta:initial-creator>
     <meta:creation-date>2003-08-12T18:15:36</meta:creation-date>
-    <dc:date>2024-03-19T23:35:51.506009158</dc:date>
+    <dc:date>2024-03-31T11:41:44.830973817</dc:date>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
-    <meta:editing-duration>PT18M8S</meta:editing-duration>
-    <meta:editing-cycles>3</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="866" meta:object-count="0"/>
+    <meta:editing-duration>PT19M52S</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="895" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">16.0300</meta:user-defined>
     <meta:user-defined meta:name="Company">RIT</meta:user-defined>
   </office:meta>
@@ -4781,12 +4864,12 @@
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Status">
               <config:config-item config:name="CursorPositionX" config:type="int">6</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">77</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">84</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">24</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">14</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">57</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -4900,108 +4983,108 @@
       <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
     </number:number-style>
     <number:number-style style:name="N125P0" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P1" style:volatile="true">
+      <number:text>-</number:text>
+      <number:fill-character> </number:fill-character>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:text> </number:text>
+    </number:number-style>
+    <number:number-style style:name="N125P2" style:volatile="true">
+      <number:text> </number:text>
+      <number:fill-character> </number:fill-character>
+      <number:text>- </number:text>
+    </number:number-style>
+    <number:text-style style:name="N125">
+      <number:text> </number:text>
+      <number:text-content/>
+      <number:text> </number:text>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
+    </number:text-style>
+    <number:number-style style:name="N121P0" style:volatile="true">
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N125">
+    <number:number-style style:name="N121">
       <number:text>-</number:text>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N125P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
     </number:number-style>
-    <number:number-style style:name="N123P0" style:volatile="true">
+    <number:time-style style:name="N120">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long" number:decimal-places="1"/>
+    </number:time-style>
+    <number:number-style style:name="N119P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N123">
+    <number:number-style style:name="N119">
       <style:text-properties fo:color="#ff0000"/>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N123P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N119P0"/>
     </number:number-style>
-    <number:time-style style:name="N122" number:truncate-on-overflow="false">
+    <number:number-style style:name="N118P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+    </number:number-style>
+    <number:number-style style:name="N118">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N118P0"/>
+    </number:number-style>
+    <number:time-style style:name="N117" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:number-style style:name="N121P0" style:volatile="true">
+    <number:number-style style:name="N116P0" style:volatile="true">
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
-    <number:number-style style:name="N121">
+    <number:number-style style:name="N116">
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N116P0"/>
     </number:number-style>
-    <number:time-style style:name="N120">
+    <number:time-style style:name="N115">
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
-    <number:number-style style:name="N119P0" style:volatile="true">
+    <number:number-style style:name="N114P0" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N119P1" style:volatile="true">
+    <number:number-style style:name="N114P1" style:volatile="true">
       <number:text>-</number:text>
       <number:fill-character> </number:fill-character>
       <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N119P2" style:volatile="true">
+    <number:number-style style:name="N114P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
       <number:text>-</number:text>
       <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N119">
+    <number:text-style style:name="N114">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N119P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N119P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N119P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N114P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N114P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N114P2"/>
     </number:text-style>
-    <number:number-style style:name="N115P0" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N115P1" style:volatile="true">
-      <number:text>-</number:text>
-      <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <number:text> </number:text>
-    </number:number-style>
-    <number:number-style style:name="N115P2" style:volatile="true">
-      <number:text> </number:text>
-      <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
-    </number:number-style>
-    <number:text-style style:name="N115">
-      <number:text> </number:text>
-      <number:text-content/>
-      <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N115P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N115P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N115P2"/>
-    </number:text-style>
-    <number:time-style style:name="N124">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long" number:decimal-places="1"/>
-    </number:time-style>
-    <number:number-style style:name="N111P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-    </number:number-style>
-    <number:number-style style:name="N111">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N111P0"/>
-    </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
       <style:table-cell-properties style:rotation-align="none" style:vertical-align="bottom"/>
       <style:text-properties style:font-name="Arial" fo:font-family="Arial" style:font-name-complex="Arial" style:font-family-complex="Arial"/>
@@ -5160,7 +5243,7 @@
         <style:region-right>
           <text:p>
             <text:span text:style-name="MT1">
-              <text:date style:data-style-name="N2" text:date-value="2024-03-19">00/00/0000</text:date>
+              <text:date style:data-style-name="N2" text:date-value="2024-03-31">00/00/0000</text:date>
             </text:span>
           </text:p>
         </style:region-right>

</xml_diff>

<commit_message>
updated status tracker and mom
</commit_message>
<xml_diff>
--- a/docs/StatusTracker3.xlsx
+++ b/docs/StatusTracker3.xlsx
@@ -99,18 +99,6 @@
     <number:text-style style:name="N100">
       <number:text-content/>
     </number:text-style>
-    <style:style style:name="ce1" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
-      <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
-    </style:style>
-    <style:style style:name="ce2" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:rotation-align="none"/>
-      <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
-    </style:style>
-    <style:style style:name="ce3" style:family="table-cell" style:parent-style-name="Default">
-      <style:table-cell-properties style:rotation-align="none"/>
-      <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
-    </style:style>
     <style:style style:name="ce13" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties style:text-align-source="fix" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties fo:text-align="center" css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
@@ -123,7 +111,7 @@
       <style:table-cell-properties style:rotation-align="none"/>
       <style:text-properties fo:color="#0000ff" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce42" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce4" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#969696" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="10pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="10pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="10pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
@@ -141,7 +129,7 @@
       <style:table-cell-properties style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="bottom" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
     </style:style>
-    <style:style style:name="ce47" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce43" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#969696" style:rotation-align="none"/>
     </style:style>
     <style:style style:name="ce9" style:family="table-cell" style:parent-style-name="Default">
@@ -160,15 +148,15 @@
       <style:table-cell-properties style:rotation-align="none"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="14pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:font-size-asian="14pt" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-name-complex="Arial1" style:font-size-complex="14pt" style:font-style-complex="normal" style:font-weight-complex="normal"/>
     </style:style>
-    <style:style style:name="ce52" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce49" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#fcf305" style:text-align-source="value-type" style:repeat-content="false" fo:wrap-option="no-wrap" style:direction="ltr" style:rotation-angle="0" style:rotation-align="none" style:shrink-to-fit="false" style:vertical-align="middle" loext:vertical-justify="auto"/>
       <style:paragraph-properties css3t:text-justify="auto" fo:margin-left="0cm" style:writing-mode="page"/>
       <style:text-properties style:use-window-font-color="true" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:font-name="Arial1" fo:font-size="12pt" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="bold" style:font-size-asian="12pt" style:font-style-asian="normal" style:font-weight-asian="bold" style:font-name-complex="Arial1" style:font-size-complex="12pt" style:font-style-complex="normal" style:font-weight-complex="bold"/>
     </style:style>
-    <style:style style:name="ce53" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce50" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#999999"/>
     </style:style>
-    <style:style style:name="ce54" style:family="table-cell" style:parent-style-name="Default">
+    <style:style style:name="ce51" style:family="table-cell" style:parent-style-name="Default">
       <style:table-cell-properties fo:background-color="#808080"/>
     </style:style>
     <style:style style:name="ce14" style:family="table-cell" style:parent-style-name="Default">
@@ -351,6 +339,9 @@
     </style:style>
     <style:style style:name="T2" style:family="text">
       <style:text-properties fo:color="#000000" loext:opacity="100%" style:text-outline="false" style:text-line-through-style="none" style:text-line-through-type="none" style:text-position="0% 100%" fo:font-family="Tahoma" style:font-family-generic="swiss" fo:font-size="8pt" fo:language="en" fo:country="IN" fo:font-style="normal" fo:text-shadow="none" style:text-underline-style="none" fo:font-weight="normal" style:text-underline-mode="continuous" style:text-overline-mode="continuous" style:text-line-through-mode="continuous" style:font-name-asian="Noto Sans CJK SC" style:font-size-asian="8pt" style:language-asian="zh" style:country-asian="CN" style:font-style-asian="normal" style:font-weight-asian="normal" style:font-family-complex="Tahoma" style:font-family-generic-complex="swiss" style:font-size-complex="8pt" style:language-complex="hi" style:country-complex="IN" style:font-style-complex="normal" style:font-weight-complex="normal" style:text-emphasize="none" style:font-relief="none" style:text-overline-style="none" style:text-overline-color="font-color"/>
+    </style:style>
+    <style:style style:name="T3" style:family="text">
+      <style:text-properties style:text-position="super 58%"/>
     </style:style>
   </office:automatic-styles>
   <office:body>
@@ -584,10 +575,10 @@
           <table:table-cell table:number-columns-repeated="1024"/>
         </table:table-row>
         <table:table-row table:style-name="ro7">
-          <table:table-cell table:style-name="ce42" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <text:p>Activity Name</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce42" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
             <text:p>Type</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce14" office:value-type="string" calcext:value-type="string">
@@ -611,7 +602,7 @@
           <table:table-cell table:style-name="ce27" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
             <text:p>Status</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce42" office:value-type="string" calcext:value-type="string">
+          <table:table-cell table:style-name="ce4" office:value-type="string" calcext:value-type="string">
             <office:annotation draw:style-name="gr2" draw:text-style-name="P2" svg:width="2.857cm" svg:height="1.252cm" svg:x="28.489cm" svg:y="3.73cm" draw:caption-point-x="4.957cm" draw:caption-point-y="-0.413cm">
               <dc:date>2024-03-01T00:00:00</dc:date>
               <text:p text:style-name="P1">
@@ -648,12 +639,12 @@
                   <text:a xlink:href="#Instructions.A1" xlink:type="simple">    See Instructions sheet for usage</text:a>
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce52" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce49" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce15" table:number-columns-repeated="3"/>
               <table:table-cell table:style-name="ce28" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce52"/>
+              <table:table-cell table:style-name="ce49"/>
               <table:table-cell table:style-name="ce15" table:number-columns-repeated="2"/>
-              <table:table-cell table:style-name="ce52" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce49" table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
               <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
@@ -663,11 +654,11 @@
                   January 21)
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce22" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce47"/>
+              <table:table-cell table:style-name="ce43"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D7]=&quot;&quot;; [.E7]=&quot;&quot;); &quot;&quot;; [.D7]-[.E7])">
                 <text:p/>
               </table:table-cell>
@@ -921,18 +912,18 @@
                   28)
                 </text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce47"/>
+              <table:table-cell table:style-name="ce43"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D17]=&quot;&quot;; [.E17]=&quot;&quot;); &quot;&quot;; [.D17]-[.E17])">
                 <text:p/>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H17]=&quot;&quot;;[.E17]=0);&quot;&quot;;ABS([.H17])/[.E17]*100)">
                 <text:p/>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
               <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1091,10 +1082,10 @@
               <table:table-cell table:number-columns-repeated="1015"/>
             </table:table-row>
             <table:table-row table:style-name="ro2">
-              <table:table-cell table:style-name="ce47" office:value-type="string" calcext:value-type="string">
+              <table:table-cell table:style-name="ce43" office:value-type="string" calcext:value-type="string">
                 <text:p>Status tracker</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+              <table:table-cell table:style-name="ce43" table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
                 <text:p>Documentation</text:p>
               </table:table-cell>
               <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -1106,14 +1097,14 @@
               <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
                 <text:p>Done</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47"/>
+              <table:table-cell table:style-name="ce43"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D24]=&quot;&quot;; [.E24]=&quot;&quot;); &quot;&quot;; [.D24]-[.E24])" office:value-type="float" office:value="0" calcext:value-type="float">
                 <text:p>0</text:p>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H24]=&quot;&quot;;[.E24]=0);&quot;&quot;;ABS([.H24])/[.E24]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
                 <text:p>0</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
             </table:table-row>
           </table:table-row-group>
         </table:table-row-group>
@@ -1176,18 +1167,18 @@
               <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
                 <text:p>Week 3 (January 29 - February 4)</text:p>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+              <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
               <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
               <table:table-cell table:style-name="ce16"/>
               <table:table-cell table:style-name="ce31" table:content-validation-name="val2"/>
-              <table:table-cell table:style-name="ce47"/>
+              <table:table-cell table:style-name="ce43"/>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D28]=&quot;&quot;; [.E28]=&quot;&quot;); &quot;&quot;; [.D28]-[.E28])">
                 <text:p/>
               </table:table-cell>
               <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H28]=&quot;&quot;;[.E28]=0);&quot;&quot;;ABS([.H28])/[.E28]*100)">
                 <text:p/>
               </table:table-cell>
-              <table:table-cell table:style-name="ce47" table:number-columns-repeated="1015"/>
+              <table:table-cell table:style-name="ce43" table:number-columns-repeated="1015"/>
             </table:table-row>
           </table:table-row-group>
         </table:table-row-group>
@@ -1342,12 +1333,12 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 4 (February 4-February 11)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce18"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce29" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce47"/>
+          <table:table-cell table:style-name="ce43"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D35]=&quot;&quot;; [.E35]=&quot;&quot;); &quot;&quot;; [.D35]-[.E35])">
             <text:p/>
           </table:table-cell>
@@ -1466,11 +1457,11 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 5 (February 11-February 18)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce32" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce47"/>
+          <table:table-cell table:style-name="ce43"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D40]=&quot;&quot;; [.E40]=&quot;&quot;); &quot;&quot;; [.D40]-[.E40])">
             <text:p/>
           </table:table-cell>
@@ -1678,11 +1669,11 @@
           <table:table-cell table:style-name="ce6" office:value-type="string" calcext:value-type="string">
             <text:p>Week 6(February 18-February 25)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce47" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce43" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce18" table:number-columns-repeated="2"/>
           <table:table-cell table:style-name="ce16"/>
           <table:table-cell table:style-name="ce33" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce47"/>
+          <table:table-cell table:style-name="ce43"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D49]=&quot;&quot;; [.E49]=&quot;&quot;); &quot;&quot;; [.D49]-[.E49])">
             <text:p/>
           </table:table-cell>
@@ -1938,10 +1929,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 7(February 25-March 2)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce50" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce53"/>
+          <table:table-cell table:style-name="ce50"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D59]=&quot;&quot;; [.E59]=&quot;&quot;); &quot;&quot;; [.D59]-[.E59])">
             <text:p/>
           </table:table-cell>
@@ -2094,10 +2085,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 8(March 2-March 9)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce50" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce53"/>
+          <table:table-cell table:style-name="ce50"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D65]=&quot;&quot;; [.E65]=&quot;&quot;); &quot;&quot;; [.D65]-[.E65])">
             <text:p/>
           </table:table-cell>
@@ -2271,10 +2262,10 @@
           <table:table-cell table:style-name="ce10" office:value-type="string" calcext:value-type="string">
             <text:p>Week 8(March 10-March 16)</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce53" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce50" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce20" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce34" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce53"/>
+          <table:table-cell table:style-name="ce50"/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D72]=&quot;&quot;; [.E72]=&quot;&quot;); &quot;&quot;; [.D72]-[.E72])">
             <text:p/>
           </table:table-cell>
@@ -2420,24 +2411,24 @@
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell table:style-name="ce46" office:value-type="string" calcext:value-type="string">
-            <text:p>Week 9(March 23-March 31)</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce54" table:content-validation-name="val1"/>
+            <text:p>Week 10(March 16-March 23)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce51" table:content-validation-name="val1"/>
           <table:table-cell table:style-name="ce58" table:number-columns-repeated="3"/>
           <table:table-cell table:style-name="ce75" table:content-validation-name="val2"/>
-          <table:table-cell table:style-name="ce54"/>
+          <table:table-cell table:style-name="ce51"/>
           <table:table-cell table:style-name="ce37" table:number-columns-repeated="2"/>
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Research on popular suggestive models</text:p>
+            <text:p>Preparation of R1 PPT</text:p>
           </table:table-cell>
           <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
             <text:p>Preparation</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Samarth,Kuvam</text:p>
+            <text:p>All members</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
             <text:p>4</text:p>
@@ -2446,7 +2437,7 @@
             <text:p>5</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
-            <text:p>Ongoing</text:p>
+            <text:p>Done</text:p>
           </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D79]=&quot;&quot;; [.E79]=&quot;&quot;); &quot;&quot;; [.D79]-[.E79])" office:value-type="float" office:value="-1" calcext:value-type="float">
@@ -2459,25 +2450,169 @@
         </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>WebCrawling for other items</text:p>
-          </table:table-cell>
-          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
-            <text:p>Development</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Anna,Kuvam</text:p>
+            <text:p>Rehersal for ppt</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Coordination</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
           <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D80]=&quot;&quot;; [.E80]=&quot;&quot;); &quot;&quot;; [.D80]-[.E80])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H80]=&quot;&quot;;[.E80]=0);&quot;&quot;;ABS([.H80])/[.E80]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>R1 eval</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="0.5" calcext:value-type="float">
+            <text:p>0.5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:number-columns-repeated="2" table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Meet with Client</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="0.5" calcext:value-type="float">
+            <text:p>0.5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Further extra features discussion</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D82]=&quot;&quot;; [.E82]=&quot;&quot;); &quot;&quot;; [.D82]-[.E82])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H82]=&quot;&quot;;[.E82]=0);&quot;&quot;;ABS([.H82])/[.E82]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Review analysis from R1 eval</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>3 to 4</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
             <text:p>Ongoing</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D80]=&quot;&quot;; [.E80]=&quot;&quot;); &quot;&quot;; [.D80]-[.E80])" office:value-type="float" office:value="0" calcext:value-type="float">
-            <text:p>0</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H80]=&quot;&quot;;[.E80]=0);&quot;&quot;;ABS([.H80])/[.E80]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H83]=&quot;&quot;;[.E83]=0);&quot;&quot;;ABS([.H83])/[.E83]*100)">
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce46" office:value-type="string" calcext:value-type="string">
+            <text:p>Week 11(March 23-March 31)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce51" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce58" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce75" table:content-validation-name="val2"/>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D84]=&quot;&quot;; [.E84]=&quot;&quot;); &quot;&quot;; [.D84]-[.E84])">
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H84]=&quot;&quot;;[.E84]=0);&quot;&quot;;ABS([.H84])/[.E84]*100)">
+            <text:p/>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Research on popular suggestive models</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
+            <text:p>4</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="5" calcext:value-type="float">
+            <text:p>5</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D85]=&quot;&quot;; [.E85]=&quot;&quot;); &quot;&quot;; [.D85]-[.E85])" office:value-type="float" office:value="-1" calcext:value-type="float">
+            <text:p>-1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H85]=&quot;&quot;;[.E85]=0);&quot;&quot;;ABS([.H85])/[.E85]*100)" office:value-type="float" office:value="20" calcext:value-type="float">
+            <text:p>20</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>WebCrawling for other items</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Anna,Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D86]=&quot;&quot;; [.E86]=&quot;&quot;); &quot;&quot;; [.D86]-[.E86])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H86]=&quot;&quot;;[.E86]=0);&quot;&quot;;ABS([.H86])/[.E86]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1015"/>
@@ -2502,8 +2637,11 @@
             <text:p>Done</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:number-columns-repeated="2" table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
-            <text:p>0</text:p>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D87]=&quot;&quot;; [.E87]=&quot;&quot;); &quot;&quot;; [.D87]-[.E87])" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H87]=&quot;&quot;;[.E87]=0);&quot;&quot;;ABS([.H87])/[.E87]*100)" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
@@ -2523,13 +2661,11 @@
           <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
             <text:p>Done</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Further extra features discussion</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D82]=&quot;&quot;; [.E82]=&quot;&quot;); &quot;&quot;; [.D82]-[.E82])" office:value-type="float" office:value="0" calcext:value-type="float">
-            <text:p>0</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H82]=&quot;&quot;;[.E82]=0);&quot;&quot;;ABS([.H82])/[.E82]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D88]=&quot;&quot;; [.E88]=&quot;&quot;); &quot;&quot;; [.D88]-[.E88])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H88]=&quot;&quot;;[.E88]=0);&quot;&quot;;ABS([.H88])/[.E88]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
             <text:p>0</text:p>
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1015"/>
@@ -2551,103 +2687,21 @@
             <text:p>Done</text:p>
           </table:table-cell>
           <table:table-cell/>
-          <table:table-cell table:style-name="ce37" office:value-type="float" office:value="0" calcext:value-type="float">
-            <text:p>0</text:p>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H83]=&quot;&quot;;[.E83]=0);&quot;&quot;;ABS([.H83])/[.E83]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
-            <text:p>0</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D84]=&quot;&quot;; [.E84]=&quot;&quot;); &quot;&quot;; [.D84]-[.E84])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H84]=&quot;&quot;;[.E84]=0);&quot;&quot;;ABS([.H84])/[.E84]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D85]=&quot;&quot;; [.E85]=&quot;&quot;); &quot;&quot;; [.D85]-[.E85])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H85]=&quot;&quot;;[.E85]=0);&quot;&quot;;ABS([.H85])/[.E85]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D86]=&quot;&quot;; [.E86]=&quot;&quot;); &quot;&quot;; [.D86]-[.E86])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H86]=&quot;&quot;;[.E86]=0);&quot;&quot;;ABS([.H86])/[.E86]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D87]=&quot;&quot;; [.E87]=&quot;&quot;); &quot;&quot;; [.D87]-[.E87])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H87]=&quot;&quot;;[.E87]=0);&quot;&quot;;ABS([.H87])/[.E87]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D88]=&quot;&quot;; [.E88]=&quot;&quot;); &quot;&quot;; [.D88]-[.E88])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H88]=&quot;&quot;;[.E88]=0);&quot;&quot;;ABS([.H88])/[.E88]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D89]=&quot;&quot;; [.E89]=&quot;&quot;); &quot;&quot;; [.D89]-[.E89])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H89]=&quot;&quot;;[.E89]=0);&quot;&quot;;ABS([.H89])/[.E89]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D89]=&quot;&quot;; [.E89]=&quot;&quot;); &quot;&quot;; [.D89]-[.E89])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H89]=&quot;&quot;;[.E89]=0);&quot;&quot;;ABS([.H89])/[.E89]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce46" office:value-type="string" calcext:value-type="string">
+            <text:p>Week 12(April 1 to April 8)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce51" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce58" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce75" table:content-validation-name="val2"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D90]=&quot;&quot;; [.E90]=&quot;&quot;); &quot;&quot;; [.D90]-[.E90])">
             <text:p/>
@@ -2658,10 +2712,22 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>View schedule page</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Anna,Vidhi</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
+            <text:p>3</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D91]=&quot;&quot;; [.E91]=&quot;&quot;); &quot;&quot;; [.D91]-[.E91])">
             <text:p/>
@@ -2672,11 +2738,25 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Add Story to Instagram(with proper image resolution)</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Have to fix the image size on story </text:p>
+          </table:table-cell>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D92]=&quot;&quot;; [.E92]=&quot;&quot;); &quot;&quot;; [.D92]-[.E92])">
             <text:p/>
           </table:table-cell>
@@ -2686,52 +2766,96 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D93]=&quot;&quot;; [.E93]=&quot;&quot;); &quot;&quot;; [.D93]-[.E93])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H93]=&quot;&quot;;[.E93]=0);&quot;&quot;;ABS([.H93])/[.E93]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D94]=&quot;&quot;; [.E94]=&quot;&quot;); &quot;&quot;; [.D94]-[.E94])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H94]=&quot;&quot;;[.E94]=0);&quot;&quot;;ABS([.H94])/[.E94]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D95]=&quot;&quot;; [.E95]=&quot;&quot;); &quot;&quot;; [.D95]-[.E95])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H95]=&quot;&quot;;[.E95]=0);&quot;&quot;;ABS([.H95])/[.E95]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Captions Updation(blogs and craft stories)</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Kuvam,Tanay</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2 to 3</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D93]=&quot;&quot;; [.E93]=&quot;&quot;); &quot;&quot;; [.D93]-[.E93])" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H93]=&quot;&quot;;[.E93]=0);&quot;&quot;;ABS([.H93])/[.E93]*100)" office:value-type="string" office:string-value="" calcext:value-type="error">
+            <text:p>#VALUE!</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Meet with Client</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              Discussed to make the final product by 15
+              <text:span text:style-name="T3">th</text:span>
+               April
+            </text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D94]=&quot;&quot;; [.E94]=&quot;&quot;); &quot;&quot;; [.D94]-[.E94])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H94]=&quot;&quot;;[.E94]=0);&quot;&quot;;ABS([.H94])/[.E94]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Changes on website to accomodate the above changes</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth,Vidhi</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D95]=&quot;&quot;; [.E95]=&quot;&quot;); &quot;&quot;; [.D95]-[.E95])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H95]=&quot;&quot;;[.E95]=0);&quot;&quot;;ABS([.H95])/[.E95]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce46" office:value-type="string" calcext:value-type="string">
+            <text:p>Week 13(April 8 to April 15)</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce51" table:content-validation-name="val1"/>
+          <table:table-cell table:style-name="ce58" table:number-columns-repeated="3"/>
+          <table:table-cell table:style-name="ce75" table:content-validation-name="val2"/>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D96]=&quot;&quot;; [.E96]=&quot;&quot;); &quot;&quot;; [.D96]-[.E96])">
             <text:p/>
@@ -2742,10 +2866,22 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Chnage in captions for blogs,craft stories</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Design</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Kuvam</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D97]=&quot;&quot;; [.E97]=&quot;&quot;); &quot;&quot;; [.D97]-[.E97])">
             <text:p/>
@@ -2756,24 +2892,47 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D98]=&quot;&quot;; [.E98]=&quot;&quot;); &quot;&quot;; [.D98]-[.E98])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H98]=&quot;&quot;;[.E98]=0);&quot;&quot;;ABS([.H98])/[.E98]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Geeting page access token for facebook</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D98]=&quot;&quot;; [.E98]=&quot;&quot;); &quot;&quot;; [.D98]-[.E98])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H98]=&quot;&quot;;[.E98]=0);&quot;&quot;;ABS([.H98])/[.E98]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Deployment of Facebook code</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Samarth</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D99]=&quot;&quot;; [.E99]=&quot;&quot;); &quot;&quot;; [.D99]-[.E99])">
             <text:p/>
@@ -2784,38 +2943,72 @@
           <table:table-cell table:number-columns-repeated="1015"/>
         </table:table-row>
         <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D100]=&quot;&quot;; [.E100]=&quot;&quot;); &quot;&quot;; [.D100]-[.E100])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H100]=&quot;&quot;;[.E100]=0);&quot;&quot;;ABS([.H100])/[.E100]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
-          <table:table-cell/>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D101]=&quot;&quot;; [.E101]=&quot;&quot;); &quot;&quot;; [.D101]-[.E101])">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H101]=&quot;&quot;;[.E101]=0);&quot;&quot;;ABS([.H101])/[.E101]*100)">
-            <text:p/>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1015"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell/>
-          <table:table-cell table:content-validation-name="val1"/>
-          <table:table-cell table:number-columns-repeated="3"/>
-          <table:table-cell table:style-name="ce30" table:content-validation-name="val2"/>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Meet with Client</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Preparation</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>All members</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D100]=&quot;&quot;; [.E100]=&quot;&quot;); &quot;&quot;; [.D100]-[.E100])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H100]=&quot;&quot;;[.E100]=0);&quot;&quot;;ABS([.H100])/[.E100]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Updation of DB for captions and new products</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Development</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Tanay</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="2" office:value-type="float" office:value="2" calcext:value-type="float">
+            <text:p>2</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Done</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D101]=&quot;&quot;; [.E101]=&quot;&quot;); &quot;&quot;; [.D101]-[.E101])" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.H101]=&quot;&quot;;[.E101]=0);&quot;&quot;;ABS([.H101])/[.E101]*100)" office:value-type="float" office:value="0" calcext:value-type="float">
+            <text:p>0</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1015"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro2">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>View posts page of meta</text:p>
+          </table:table-cell>
+          <table:table-cell table:content-validation-name="val1" office:value-type="string" calcext:value-type="string">
+            <text:p>Design</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Anna</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>1.5 to 2</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+          <table:table-cell table:style-name="ce30" table:content-validation-name="val2" office:value-type="string" calcext:value-type="string">
+            <text:p>Ongoing</text:p>
+          </table:table-cell>
           <table:table-cell/>
           <table:table-cell table:style-name="ce37" table:formula="of:=IF(OR([.D102]=&quot;&quot;; [.E102]=&quot;&quot;); &quot;&quot;; [.D102]-[.E102])">
             <text:p/>
@@ -4825,11 +5018,11 @@
   <office:meta>
     <meta:initial-creator>swami</meta:initial-creator>
     <meta:creation-date>2003-08-12T18:15:36</meta:creation-date>
-    <dc:date>2024-03-31T11:41:44.830973817</dc:date>
+    <dc:date>2024-04-10T16:45:15.247587676</dc:date>
     <meta:generator>LibreOffice/7.3.7.2$Linux_X86_64 LibreOffice_project/30$Build-2</meta:generator>
-    <meta:editing-duration>PT19M52S</meta:editing-duration>
-    <meta:editing-cycles>5</meta:editing-cycles>
-    <meta:document-statistic meta:table-count="2" meta:cell-count="895" meta:object-count="0"/>
+    <meta:editing-duration>PT23M34S</meta:editing-duration>
+    <meta:editing-cycles>6</meta:editing-cycles>
+    <meta:document-statistic meta:table-count="2" meta:cell-count="990" meta:object-count="0"/>
     <meta:user-defined meta:name="AppVersion">16.0300</meta:user-defined>
     <meta:user-defined meta:name="Company">RIT</meta:user-defined>
   </office:meta>
@@ -4864,12 +5057,12 @@
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="Status">
               <config:config-item config:name="CursorPositionX" config:type="int">6</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">84</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">101</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">24</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">57</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">63</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -4934,7 +5127,7 @@
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
       <config:config-item config:name="PrinterName" config:type="string">Generic Printer</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">oAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKRHVwbGV4Ok5vbmUAUGFnZVNpemU6QTQAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">oAH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwQAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luYWRqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4dERhdGEKUGFnZVNpemU6QTQARHVwbGV4Ok5vbmUAABIAQ09NUEFUX0RVUExFWF9NT0RFDwBEdXBsZXhNb2RlOjpPZmY=</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1000</config:config-item>
@@ -4979,112 +5172,112 @@
     <number:number-style style:name="N0">
       <number:number number:min-integer-digits="1"/>
     </number:number-style>
-    <number:number-style style:name="N126">
-      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
-    </number:number-style>
-    <number:number-style style:name="N125P0" style:volatile="true">
+    <number:number-style style:name="N126P0" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N125P1" style:volatile="true">
+    <number:number-style style:name="N126P1" style:volatile="true">
       <number:text>-</number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N125P2" style:volatile="true">
+    <number:number-style style:name="N126P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:text>- </number:text>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
+      <number:text> </number:text>
     </number:number-style>
-    <number:text-style style:name="N125">
+    <number:text-style style:name="N126">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N125P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N125P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N125P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N126P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N126P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N126P2"/>
     </number:text-style>
+    <number:time-style style:name="N122">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long"/>
+    </number:time-style>
     <number:number-style style:name="N121P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
     <number:number-style style:name="N121">
       <number:text>-</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N121P0"/>
     </number:number-style>
-    <number:time-style style:name="N120">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long" number:decimal-places="1"/>
-    </number:time-style>
-    <number:number-style style:name="N119P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-    </number:number-style>
-    <number:number-style style:name="N119">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N119P0"/>
-    </number:number-style>
-    <number:number-style style:name="N118P0" style:volatile="true">
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-    </number:number-style>
-    <number:number-style style:name="N118">
-      <style:text-properties fo:color="#ff0000"/>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
-      <style:map style:condition="value()&gt;=0" style:apply-style-name="N118P0"/>
-    </number:number-style>
-    <number:time-style style:name="N117" number:truncate-on-overflow="false">
+    <number:time-style style:name="N120" number:truncate-on-overflow="false">
       <number:hours/>
       <number:text>:</number:text>
       <number:minutes number:style="long"/>
       <number:text>:</number:text>
       <number:seconds number:style="long"/>
     </number:time-style>
+    <number:number-style style:name="N119P0" style:volatile="true">
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+    </number:number-style>
+    <number:number-style style:name="N119">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N119P0"/>
+    </number:number-style>
+    <number:number-style style:name="N118P0" style:volatile="true">
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+    </number:number-style>
+    <number:number-style style:name="N118">
+      <style:text-properties fo:color="#ff0000"/>
+      <number:text>-</number:text>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <style:map style:condition="value()&gt;=0" style:apply-style-name="N118P0"/>
+    </number:number-style>
+    <number:time-style style:name="N117">
+      <number:minutes number:style="long"/>
+      <number:text>:</number:text>
+      <number:seconds number:style="long" number:decimal-places="1"/>
+    </number:time-style>
     <number:number-style style:name="N116P0" style:volatile="true">
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
     </number:number-style>
     <number:number-style style:name="N116">
       <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
       <style:map style:condition="value()&gt;=0" style:apply-style-name="N116P0"/>
     </number:number-style>
-    <number:time-style style:name="N115">
-      <number:minutes number:style="long"/>
-      <number:text>:</number:text>
-      <number:seconds number:style="long"/>
-    </number:time-style>
-    <number:number-style style:name="N114P0" style:volatile="true">
+    <number:number-style style:name="N115P0" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N114P1" style:volatile="true">
+    <number:number-style style:name="N115P1" style:volatile="true">
       <number:text>-</number:text>
       <number:fill-character> </number:fill-character>
-      <number:number number:decimal-places="2" number:min-decimal-places="2" number:min-integer-digits="1" number:grouping="true"/>
+      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="1" number:grouping="true"/>
       <number:text> </number:text>
     </number:number-style>
-    <number:number-style style:name="N114P2" style:volatile="true">
+    <number:number-style style:name="N115P2" style:volatile="true">
       <number:text> </number:text>
       <number:fill-character> </number:fill-character>
-      <number:text>-</number:text>
-      <number:number number:decimal-places="0" number:min-decimal-places="0" number:min-integer-digits="0"/>
-      <number:text> </number:text>
+      <number:text>- </number:text>
     </number:number-style>
-    <number:text-style style:name="N114">
+    <number:text-style style:name="N115">
       <number:text> </number:text>
       <number:text-content/>
       <number:text> </number:text>
-      <style:map style:condition="value()&gt;0" style:apply-style-name="N114P0"/>
-      <style:map style:condition="value()&lt;0" style:apply-style-name="N114P1"/>
-      <style:map style:condition="value()=0" style:apply-style-name="N114P2"/>
+      <style:map style:condition="value()&gt;0" style:apply-style-name="N115P0"/>
+      <style:map style:condition="value()&lt;0" style:apply-style-name="N115P1"/>
+      <style:map style:condition="value()=0" style:apply-style-name="N115P2"/>
     </number:text-style>
+    <number:number-style style:name="N111">
+      <number:scientific-number number:decimal-places="1" number:min-decimal-places="1" number:min-integer-digits="1" number:min-exponent-digits="1" number:exponent-interval="3" number:forced-exponent-sign="true"/>
+    </number:number-style>
     <style:style style:name="Default" style:family="table-cell">
       <style:table-cell-properties style:rotation-align="none" style:vertical-align="bottom"/>
       <style:text-properties style:font-name="Arial" fo:font-family="Arial" style:font-name-complex="Arial" style:font-family-complex="Arial"/>
@@ -5243,7 +5436,7 @@
         <style:region-right>
           <text:p>
             <text:span text:style-name="MT1">
-              <text:date style:data-style-name="N2" text:date-value="2024-03-31">00/00/0000</text:date>
+              <text:date style:data-style-name="N2" text:date-value="2024-04-10">00/00/0000</text:date>
             </text:span>
           </text:p>
         </style:region-right>

</xml_diff>